<commit_message>
Another iteration of the PCB and made some updates to the BOM
</commit_message>
<xml_diff>
--- a/Eye Diagram PCB BOM.xlsx
+++ b/Eye Diagram PCB BOM.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammolnar/Desktop/ATLAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammolnar/Desktop/ATLAS/Custom_PCB_Eye_Diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A9BA5F-22E1-E44E-B9F5-DE2527430CC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F3A2F5-207E-784D-93A0-82F7635452AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="460" windowWidth="32740" windowHeight="20540" xr2:uid="{FFA9E2BE-5311-4046-8D37-80F8AA747451}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="32880" windowHeight="20540" xr2:uid="{FFA9E2BE-5311-4046-8D37-80F8AA747451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="120">
   <si>
     <t>Item #</t>
   </si>
@@ -68,15 +60,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>C1, C2, C4, C5, C11, C12, C13, C14, C15, C16, C17, C18</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C6, C7, C8, C9, C10</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9</t>
   </si>
   <si>
@@ -89,30 +72,12 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>J1, J4</t>
-  </si>
-  <si>
-    <t>J2, J7, J8, J9, J12, J13</t>
-  </si>
-  <si>
-    <t>J3, J5</t>
-  </si>
-  <si>
     <t>J6</t>
   </si>
   <si>
     <t>J10</t>
   </si>
   <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>J14, J15</t>
-  </si>
-  <si>
-    <t>J16, J17</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -194,12 +159,6 @@
     <t>Taiyo Yuden</t>
   </si>
   <si>
-    <t>DSC1123CI2-125.0000</t>
-  </si>
-  <si>
-    <t>576-4648-ND</t>
-  </si>
-  <si>
     <t>Microchip Technology</t>
   </si>
   <si>
@@ -260,18 +219,6 @@
     <t>CONN PWR JACK 2.5X5.5MM SOLDER</t>
   </si>
   <si>
-    <t>Adam Tech</t>
-  </si>
-  <si>
-    <t>PH1-01-UA</t>
-  </si>
-  <si>
-    <t>2057-PH1-01-UA-ND</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 1POS 2.54MM</t>
-  </si>
-  <si>
     <t>M20-8890445</t>
   </si>
   <si>
@@ -323,12 +270,6 @@
     <t>Murata Power Solutions Inc.</t>
   </si>
   <si>
-    <t>OKI-78SR-3.3/1.5-W36H-C</t>
-  </si>
-  <si>
-    <t>811-3014-ND</t>
-  </si>
-  <si>
     <t>LSHM-150-04.0-L-DV-A-S-K-TR</t>
   </si>
   <si>
@@ -341,21 +282,6 @@
     <t>DC DC CONVERTER 3.3V 5W</t>
   </si>
   <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
-    <t>SML-D12U1WT86</t>
-  </si>
-  <si>
-    <t>SML-D12U1WT86CT-ND</t>
-  </si>
-  <si>
-    <t>2.2 Vf</t>
-  </si>
-  <si>
-    <t>LED RED DIFFUSED 1608 SMD</t>
-  </si>
-  <si>
     <t>RC0402FR-07330RL</t>
   </si>
   <si>
@@ -393,6 +319,72 @@
   </si>
   <si>
     <t>811-2195-5-ND</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C6, C10,</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C2, C4, C8, C9, C11, C12, C13, C14, C15, C16, C17, C18</t>
+  </si>
+  <si>
+    <t>1x02</t>
+  </si>
+  <si>
+    <t>J9, J13</t>
+  </si>
+  <si>
+    <t>Molex Connector</t>
+  </si>
+  <si>
+    <t>J1, J4, J7, J8, J11, J12, J15, J17</t>
+  </si>
+  <si>
+    <t>LSHM Connector</t>
+  </si>
+  <si>
+    <t>J14, J16</t>
+  </si>
+  <si>
+    <t>1x03</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>Power Connector</t>
+  </si>
+  <si>
+    <t>1x04</t>
+  </si>
+  <si>
+    <t>J5, J2</t>
+  </si>
+  <si>
+    <t>OSRAM Opto Semiconductors Inc.</t>
+  </si>
+  <si>
+    <t>2v</t>
+  </si>
+  <si>
+    <t>475-2761-1-ND</t>
+  </si>
+  <si>
+    <t>LS L296-P2Q2-1-Z</t>
+  </si>
+  <si>
+    <t>Red 630nm LED Indication - Discrete 2V 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>DSC1123CI2-125.0000T</t>
+  </si>
+  <si>
+    <t>DSC1123CI2-125.0000TCT-ND</t>
   </si>
 </sst>
 </file>
@@ -414,18 +406,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -449,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,8 +449,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA906EB-A519-B443-9B99-E6B38EFFBFEE}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,9 +774,11 @@
     <col min="3" max="3" width="45.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.83203125" customWidth="1"/>
-    <col min="6" max="7" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -837,26 +823,26 @@
       <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>402</v>
@@ -870,25 +856,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J3">
         <v>402</v>
@@ -902,61 +888,62 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>805</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="5">
         <v>603</v>
       </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -966,25 +953,25 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J6">
         <v>603</v>
@@ -998,50 +985,53 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J7">
         <v>603</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1051,19 +1041,22 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4">
         <v>472720024</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1071,25 +1064,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1100,22 +1096,25 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1126,22 +1125,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1152,25 +1154,28 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E13" s="4">
         <v>878321420</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1181,167 +1186,179 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="4">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="5">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="4">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5">
-        <v>2</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" s="5">
+      <c r="J18">
         <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J19">
         <v>402</v>
@@ -1349,31 +1366,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J20">
         <v>402</v>
@@ -1381,84 +1398,32 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21">
-        <v>402</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
       <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>21</v>
-      </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
+        <f>SUM(B2:B21)</f>
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>